<commit_message>
fix #99 + minor
</commit_message>
<xml_diff>
--- a/uem.basesDeDatos.alonsostein.git/MinimumBalance.xlsx
+++ b/uem.basesDeDatos.alonsostein.git/MinimumBalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -353,7 +353,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.99</v>
+        <v>19.989999999999998</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
min balance WORKAROUND related to issue #101
</commit_message>
<xml_diff>
--- a/uem.basesDeDatos.alonsostein.git/MinimumBalance.xlsx
+++ b/uem.basesDeDatos.alonsostein.git/MinimumBalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>19.989999999999998</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nicer min balance for demo
</commit_message>
<xml_diff>
--- a/uem.basesDeDatos.alonsostein.git/MinimumBalance.xlsx
+++ b/uem.basesDeDatos.alonsostein.git/MinimumBalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>19.7</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>